<commit_message>
Data insertion to the Database MySQl
</commit_message>
<xml_diff>
--- a/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
+++ b/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCS FAST NUCES\Semesters Data\8th Sem\Data Mining\Assignments\Assignment2\TechStackDiary\data-engineering\DE_projects\2024_p1_retail-data-engineering\docs\src_data_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0D8A43A-FA87-4F00-9BA5-5B6FBBF0FB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F260C-719C-48ED-ACA4-76F92C078E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
   </bookViews>
@@ -391,9 +391,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -407,6 +404,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,117 +724,117 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="27.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to the SRC Data Mapping Sheet
</commit_message>
<xml_diff>
--- a/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
+++ b/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCS FAST NUCES\Semesters Data\8th Sem\Data Mining\Assignments\Assignment2\TechStackDiary\data-engineering\DE_projects\2024_p1_retail-data-engineering\docs\src_data_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F260C-719C-48ED-ACA4-76F92C078E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF227F89-26EA-457F-96E8-47DDBC94488E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
   </bookViews>
   <sheets>
     <sheet name="SrcsSummary" sheetId="1" r:id="rId1"/>
+    <sheet name="CRM_System" sheetId="2" r:id="rId2"/>
+    <sheet name="Inventory_mgmt_sys" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
   <si>
     <t>System</t>
   </si>
@@ -313,12 +315,171 @@
   <si>
     <t>MySQL</t>
   </si>
+  <si>
+    <t>Database Name</t>
+  </si>
+  <si>
+    <t>CRM_System</t>
+  </si>
+  <si>
+    <t>rizwanhaidar</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>qaws123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customers </t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object </t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>loyalty_points</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>DataType</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>DataType Length</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Inventory_mgmt_sys</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>unit_price</t>
+  </si>
+  <si>
+    <t>cost_price</t>
+  </si>
+  <si>
+    <t>supplier_id</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>ENUM</t>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>Nullable</t>
+  </si>
+  <si>
+    <t>DEFAULT Value</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('Electronics', 'Clothing', 'Home &amp; Kitchen', 'Books', 'Toys') </t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>chk_price CHECK (cost_price &lt;= unit_price)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +507,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -361,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -384,11 +553,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -407,11 +661,510 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -422,6 +1175,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5994ED9-E527-4C19-97AD-4C41341ED63B}" name="Table1" displayName="Table1" ref="A5:H12" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
+  <autoFilter ref="A5:H12" xr:uid="{F5994ED9-E527-4C19-97AD-4C41341ED63B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B88540F1-C782-4FB9-90A3-55CA4276F9C5}" name="Database" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{0C9739C9-2D50-4088-BD26-ADC72A63635B}" name="Object " dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{F87BCA9A-FBD3-4254-98D1-A6A97378641D}" name="Fields" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{E6DCAD66-2727-46AF-8417-79B348862884}" name="DataType" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{B6F65419-4DDD-4D9E-8E3E-9599E82A5534}" name="DataType Length" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{5C068E9E-6DD8-40CB-AA72-EE1191194D8A}" name="Precision" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{8CCF80A7-7E35-4C2C-806A-3B0F8945D9AD}" name="PK" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{D6381F83-E0CF-43E8-93F4-761A246A569E}" name="PI" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B75B5F5D-BC5F-4B2A-A276-7E433DABA8F3}" name="Table13" displayName="Table13" ref="A5:L18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A5:L18" xr:uid="{B75B5F5D-BC5F-4B2A-A276-7E433DABA8F3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{A4D39252-A8C0-4506-8249-F506E8B7AA0E}" name="Database" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{402BF4D3-A06D-468E-969B-1D9B7F9ED9B4}" name="Object " dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{10BD143D-C747-4A8A-A1FD-C086FD2D3621}" name="Fields" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{95DFA97B-A3AE-454D-B58B-8DEF031ABEC9}" name="DataType" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{9C2B576C-929E-401E-9F54-55396B5D9169}" name="DataType Length" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{ACBC2FFB-2AE2-4638-8BAA-B651CEDCE8A9}" name="Precision" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{6542E1E0-EAD3-4D67-83A2-8EDBDB9FC194}" name="DEFAULT Value" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{99160C91-78CC-4102-BBE2-2FBFF40C4119}" name="Nullable" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{CDFBAF00-473A-48EC-A4FE-9EDC3E99B37F}" name="Unique" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{73A15B07-509B-4704-B069-850B50E450C1}" name="PK" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{6CBFF587-3C0C-4FFB-99F6-F2FBDF3ECD52}" name="PI" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6AE01E21-F22A-48A2-BEB5-D60C01494486}" name="Constraints" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -723,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE0FB0E-4018-4F07-9D4A-5354A6C31BA4}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -844,4 +1635,787 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0157817F-A9D7-43DF-95E3-E40220436C38}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="9">
+        <v>36</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="9">
+        <v>50</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9">
+        <v>50</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="9">
+        <v>100</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="9">
+        <v>20</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="9">
+        <v>255</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0B2AA3-45F5-487C-B678-A89EC6F4F6A8}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="24.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="21">
+        <v>36</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="21">
+        <v>255</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="21">
+        <v>255</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="29"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="21">
+        <v>10</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="21">
+        <v>10</v>
+      </c>
+      <c r="F11" s="21">
+        <v>2</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="29"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="21">
+        <v>36</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="29"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="21">
+        <v>50</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="21">
+        <v>255</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="29"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="21">
+        <v>5</v>
+      </c>
+      <c r="F16" s="21">
+        <v>2</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="21">
+        <v>50</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Supplier Data Creation & Bridging with Products
</commit_message>
<xml_diff>
--- a/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
+++ b/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCS FAST NUCES\Semesters Data\8th Sem\Data Mining\Assignments\Assignment2\TechStackDiary\data-engineering\DE_projects\2024_p1_retail-data-engineering\docs\src_data_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14CD720-09BF-48AF-913B-E5A11626906E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19FFE03-917C-4D27-ABD6-A118930CD979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="76">
   <si>
     <t>System</t>
   </si>
@@ -130,73 +130,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>returns.avro</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>products</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inventory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>suppliers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>customers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>loyalty_program</t>
     </r>
   </si>
   <si>
@@ -506,12 +439,99 @@
     CONSTRAINT chk_price CHECK (cost_price &lt;= unit_price)  -- Ensures cost price is not higher than unit price
 );</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>customers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>loyalty_program</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>products</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inventory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>suppliers</t>
+    </r>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +572,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -784,16 +812,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -807,97 +835,17 @@
   <dxfs count="34">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -906,7 +854,77 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1023,13 +1041,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1047,6 +1058,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1163,7 +1181,7 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1176,11 +1194,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1193,11 +1213,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1210,11 +1232,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1227,11 +1251,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1244,6 +1270,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1321,42 +1349,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67FDEBFB-E9DC-4EF7-86C5-3F0FE67956BF}" name="Table134" displayName="Table134" ref="A6:L13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67FDEBFB-E9DC-4EF7-86C5-3F0FE67956BF}" name="Table134" displayName="Table134" ref="A6:L13" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A6:L13" xr:uid="{67FDEBFB-E9DC-4EF7-86C5-3F0FE67956BF}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D116019C-B02D-4589-AAA3-D1F6EC74C6F1}" name="Database" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7ED60EFF-9781-4D1A-BA26-AD048E45B0FE}" name="Object " dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{95FB723E-9B0B-4E45-B7C8-B142E2C7B373}" name="Fields" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{880CF212-7549-40AA-AA52-B2A2CABCF6B8}" name="DataType" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A7846B4F-9536-4856-AD7C-FCDDCD49241C}" name="DataType Length" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{28545C28-B506-468E-98C4-28B2DEC8363B}" name="Precision" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{4F1A8760-3567-4163-8A5B-A2E8908A3595}" name="DEFAULT Value" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{E4E6768B-E8BC-44E3-BB8C-74DFF47C3F51}" name="Nullable" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{E9C07FB5-D637-4857-8B85-56CBEEF43FC3}" name="Unique" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{9BBC9B25-D59E-4882-A285-0D64DC0E6579}" name="PK" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{36267D32-4A24-4861-AAF4-D18A5B4AE626}" name="PI" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{781C2982-ED36-484D-AAC0-3CA8846A3360}" name="Constraints" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{D116019C-B02D-4589-AAA3-D1F6EC74C6F1}" name="Database" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{7ED60EFF-9781-4D1A-BA26-AD048E45B0FE}" name="Object " dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{95FB723E-9B0B-4E45-B7C8-B142E2C7B373}" name="Fields" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{880CF212-7549-40AA-AA52-B2A2CABCF6B8}" name="DataType" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{A7846B4F-9536-4856-AD7C-FCDDCD49241C}" name="DataType Length" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{28545C28-B506-468E-98C4-28B2DEC8363B}" name="Precision" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{4F1A8760-3567-4163-8A5B-A2E8908A3595}" name="DEFAULT Value" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{E4E6768B-E8BC-44E3-BB8C-74DFF47C3F51}" name="Nullable" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{E9C07FB5-D637-4857-8B85-56CBEEF43FC3}" name="Unique" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{9BBC9B25-D59E-4882-A285-0D64DC0E6579}" name="PK" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{36267D32-4A24-4861-AAF4-D18A5B4AE626}" name="PI" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{781C2982-ED36-484D-AAC0-3CA8846A3360}" name="Constraints" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B75B5F5D-BC5F-4B2A-A276-7E433DABA8F3}" name="Table13" displayName="Table13" ref="A6:L19" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B75B5F5D-BC5F-4B2A-A276-7E433DABA8F3}" name="Table13" displayName="Table13" ref="A6:L19" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A6:L19" xr:uid="{B75B5F5D-BC5F-4B2A-A276-7E433DABA8F3}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A4D39252-A8C0-4506-8249-F506E8B7AA0E}" name="Database" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{402BF4D3-A06D-468E-969B-1D9B7F9ED9B4}" name="Object " dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{10BD143D-C747-4A8A-A1FD-C086FD2D3621}" name="Fields" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{95DFA97B-A3AE-454D-B58B-8DEF031ABEC9}" name="DataType" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{9C2B576C-929E-401E-9F54-55396B5D9169}" name="DataType Length" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{ACBC2FFB-2AE2-4638-8BAA-B651CEDCE8A9}" name="Precision" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{6542E1E0-EAD3-4D67-83A2-8EDBDB9FC194}" name="DEFAULT Value" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{99160C91-78CC-4102-BBE2-2FBFF40C4119}" name="Nullable" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{CDFBAF00-473A-48EC-A4FE-9EDC3E99B37F}" name="Unique" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{73A15B07-509B-4704-B069-850B50E450C1}" name="PK" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{6CBFF587-3C0C-4FFB-99F6-F2FBDF3ECD52}" name="PI" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{6AE01E21-F22A-48A2-BEB5-D60C01494486}" name="Constraints" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{A4D39252-A8C0-4506-8249-F506E8B7AA0E}" name="Database" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{402BF4D3-A06D-468E-969B-1D9B7F9ED9B4}" name="Object " dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{10BD143D-C747-4A8A-A1FD-C086FD2D3621}" name="Fields" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{95DFA97B-A3AE-454D-B58B-8DEF031ABEC9}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{9C2B576C-929E-401E-9F54-55396B5D9169}" name="DataType Length" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{ACBC2FFB-2AE2-4638-8BAA-B651CEDCE8A9}" name="Precision" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{6542E1E0-EAD3-4D67-83A2-8EDBDB9FC194}" name="DEFAULT Value" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{99160C91-78CC-4102-BBE2-2FBFF40C4119}" name="Nullable" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{CDFBAF00-473A-48EC-A4FE-9EDC3E99B37F}" name="Unique" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{73A15B07-509B-4704-B069-850B50E450C1}" name="PK" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{6CBFF587-3C0C-4FFB-99F6-F2FBDF3ECD52}" name="PI" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{6AE01E21-F22A-48A2-BEB5-D60C01494486}" name="Constraints" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1662,7 +1690,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,12 +1703,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1693,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1716,10 +1744,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1730,10 +1758,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1741,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1756,10 +1784,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1770,10 +1798,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1811,37 +1839,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>71</v>
+      <c r="A5" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -1854,59 +1882,59 @@
       <c r="K5" s="27"/>
       <c r="L5" s="28"/>
       <c r="M5" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>41</v>
-      </c>
       <c r="K6" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="8">
         <v>36</v>
@@ -1918,25 +1946,25 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="8">
         <v>50</v>
@@ -1948,25 +1976,25 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="8">
         <v>50</v>
@@ -1978,25 +2006,25 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8">
         <v>100</v>
@@ -2008,25 +2036,25 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="8">
         <v>20</v>
@@ -2038,25 +2066,25 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="8">
         <v>255</v>
@@ -2068,25 +2096,25 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9">
@@ -2096,10 +2124,10 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L13" s="20"/>
     </row>
@@ -2130,38 +2158,38 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>71</v>
+      <c r="A5" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -2176,54 +2204,54 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>41</v>
-      </c>
       <c r="K6" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="D7" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" s="14">
         <v>36</v>
@@ -2233,33 +2261,33 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="D8" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="14">
         <v>255</v>
@@ -2269,65 +2297,65 @@
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14">
         <v>0</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="14">
         <v>255</v>
@@ -2337,31 +2365,31 @@
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="14">
         <v>10</v>
@@ -2371,31 +2399,31 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="14">
         <v>10</v>
@@ -2405,31 +2433,31 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="14">
         <v>36</v>
@@ -2439,31 +2467,31 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="14">
         <v>50</v>
@@ -2471,61 +2499,61 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" s="14">
         <v>255</v>
@@ -2533,31 +2561,31 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="14">
         <v>5</v>
@@ -2567,31 +2595,31 @@
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="14">
         <v>50</v>
@@ -2599,31 +2627,31 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
@@ -2631,16 +2659,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L19" s="22"/>
     </row>

</xml_diff>

<commit_message>
Added code for Bulk Transaction Data Generation
</commit_message>
<xml_diff>
--- a/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
+++ b/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCS FAST NUCES\Semesters Data\8th Sem\Data Mining\Assignments\Assignment2\TechStackDiary\data-engineering\DE_projects\2024_p1_retail-data-engineering\docs\src_data_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19FFE03-917C-4D27-ABD6-A118930CD979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAF3A3-3C9B-4311-8479-A97336C889B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
   </bookViews>
@@ -72,68 +72,6 @@
   </si>
   <si>
     <r>
-      <t>transactions.csv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>transactions.avro</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>returns.csv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>returns.avro</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>online_orders.parquet</t>
     </r>
     <r>
@@ -525,6 +463,78 @@
   </si>
   <si>
     <t>SQL Server</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transactions.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transactions.avro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>returns.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>returns.avro</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1690,7 +1700,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1729,7 +1739,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -1744,10 +1754,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1758,10 +1768,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1769,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1784,10 +1794,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
@@ -1798,10 +1808,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1809,6 +1819,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1839,26 +1850,26 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1866,10 +1877,10 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>70</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -1882,59 +1893,59 @@
       <c r="K5" s="27"/>
       <c r="L5" s="28"/>
       <c r="M5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>39</v>
-      </c>
       <c r="K6" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8">
         <v>36</v>
@@ -1946,25 +1957,25 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="8">
         <v>50</v>
@@ -1976,25 +1987,25 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8">
         <v>50</v>
@@ -2006,25 +2017,25 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="8">
         <v>100</v>
@@ -2036,25 +2047,25 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="8">
         <v>20</v>
@@ -2066,25 +2077,25 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="8">
         <v>255</v>
@@ -2096,25 +2107,25 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9">
@@ -2124,10 +2135,10 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L13" s="20"/>
     </row>
@@ -2158,26 +2169,26 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2186,10 +2197,10 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -2204,54 +2215,54 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>39</v>
-      </c>
       <c r="K6" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>45</v>
-      </c>
       <c r="D7" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="14">
         <v>36</v>
@@ -2261,33 +2272,33 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C8" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="14">
         <v>255</v>
@@ -2297,65 +2308,65 @@
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14">
         <v>0</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="14">
         <v>255</v>
@@ -2365,31 +2376,31 @@
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C11" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="14">
         <v>10</v>
@@ -2399,31 +2410,31 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="14">
         <v>10</v>
@@ -2433,31 +2444,31 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="14">
         <v>36</v>
@@ -2467,31 +2478,31 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="14">
         <v>50</v>
@@ -2499,61 +2510,61 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C15" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="14">
         <v>255</v>
@@ -2561,31 +2572,31 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="14">
         <v>5</v>
@@ -2595,31 +2606,31 @@
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C18" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="14">
         <v>50</v>
@@ -2627,31 +2638,31 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C19" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
@@ -2659,16 +2670,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L19" s="22"/>
     </row>

</xml_diff>

<commit_message>
Data Creation Store Management
1. Added Python code to create data for Employees and Stores
2. Added SQL code to create tables in SSMS
3. Added SQL Code to make some updates and perform data consistency checks
</commit_message>
<xml_diff>
--- a/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
+++ b/data-engineering/DE_projects/2024_p1_retail-data-engineering/docs/src_data_information/source_metadata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCS FAST NUCES\Semesters Data\8th Sem\Data Mining\Assignments\Assignment2\TechStackDiary\data-engineering\DE_projects\2024_p1_retail-data-engineering\docs\src_data_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAF3A3-3C9B-4311-8479-A97336C889B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F268ED-2B99-45C9-B0A0-06E48AFF58A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{69848CC2-1893-441E-8429-C0456A83DEE8}"/>
   </bookViews>
   <sheets>
     <sheet name="SrcsSummary" sheetId="1" r:id="rId1"/>
-    <sheet name="CRM_System" sheetId="2" r:id="rId2"/>
-    <sheet name="Inventory_mgmt_sys" sheetId="3" r:id="rId3"/>
+    <sheet name="POS_System" sheetId="4" r:id="rId2"/>
+    <sheet name="CRM_System" sheetId="2" r:id="rId3"/>
+    <sheet name="Inventory_mgmt_sys" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1824,6 +1825,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18226FCA-F483-41D8-9939-4E1C53FFBA30}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0157817F-A9D7-43DF-95E3-E40220436C38}">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -2154,7 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0B2AA3-45F5-487C-B678-A89EC6F4F6A8}">
   <dimension ref="A1:L19"/>
   <sheetViews>

</xml_diff>